<commit_message>
units out of raw detection template
</commit_message>
<xml_diff>
--- a/Load/ontology/label_templates/raw_detection_template.xlsx
+++ b/Load/ontology/label_templates/raw_detection_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/label_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54825C02-AE46-614A-9D5E-E1DA93E6CC4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA39983-6722-324C-81FB-45CFA028C59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_detection_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>variable</t>
   </si>
@@ -123,6 +127,18 @@
       </rPr>
       <t>Then, enter any additional specifics from data provider (serotype, gene) UNLESS species is E. coli.</t>
     </r>
+  </si>
+  <si>
+    <t>TAC</t>
+  </si>
+  <si>
+    <t>Ct value</t>
+  </si>
+  <si>
+    <t>Virus</t>
+  </si>
+  <si>
+    <t>Dengue</t>
   </si>
 </sst>
 </file>
@@ -981,7 +997,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,6 +1101,24 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="N3" s="2" t="str">
         <f>TRIM(IF($H3="",$G3,"")
 &amp;IF($H3&lt;&gt;"",$H3,"")
@@ -1093,12 +1127,12 @@
 &amp;IF($K3&lt;&gt;""," "&amp;$K3,"")
 &amp;IF($J3&lt;&gt;""," "&amp;$J3&amp;"-pos","")
 &amp;IF($L3&lt;&gt;""," "&amp;$L3&amp;"-neg","")
-&amp;IF($D3&lt;&gt;""," "&amp;$D3,"")&amp;", by "&amp;$C3&amp;" result")</f>
-        <v>, by result</v>
+&amp;", by "&amp;$C3&amp;" result")</f>
+        <v>Dengue, by TAC result</v>
       </c>
       <c r="O3" s="2" t="str">
         <f>TRIM("Raw "&amp;LOWER($E3)&amp;" data for "&amp;$B3)</f>
-        <v>Raw data for</v>
+        <v>Raw virus data for stool</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="81" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
minor adjustments to raw_detection_template
make clear where to enter unitLabel
</commit_message>
<xml_diff>
--- a/Load/ontology/label_templates/raw_detection_template.xlsx
+++ b/Load/ontology/label_templates/raw_detection_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/label_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA39983-6722-324C-81FB-45CFA028C59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE251B8-D005-4B48-8C32-084CE33D7105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>variable</t>
   </si>
@@ -43,9 +43,6 @@
     <t>assay type</t>
   </si>
   <si>
-    <t>website label</t>
-  </si>
-  <si>
     <t>domain</t>
   </si>
   <si>
@@ -64,15 +61,9 @@
     <t>&lt;--INPUT | OUTPUT --&gt;</t>
   </si>
   <si>
-    <t>website parent</t>
-  </si>
-  <si>
     <t>stool</t>
   </si>
   <si>
-    <t>value specification</t>
-  </si>
-  <si>
     <t>E.g.: bacteriology, TAC, ELISA, … . Leave blank for MALED aggregate data.</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
   </si>
   <si>
     <t>enterotoxic or virulence factor tested negative</t>
-  </si>
-  <si>
-    <t>e.g. Ct value</t>
   </si>
   <si>
     <t>Parent term in ClinEpi</t>
@@ -139,6 +127,15 @@
   </si>
   <si>
     <t>Dengue</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>parentLabel</t>
+  </si>
+  <si>
+    <t>unitLabel</t>
   </si>
 </sst>
 </file>
@@ -991,13 +988,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,28 +1002,27 @@
     <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="22.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="23.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="30.33203125" style="2" customWidth="1"/>
-    <col min="15" max="16" width="18.33203125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="17.1640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="15.5" style="2" customWidth="1"/>
-    <col min="20" max="20" width="24.5" style="2" customWidth="1"/>
-    <col min="21" max="21" width="18" style="2" customWidth="1"/>
-    <col min="22" max="22" width="42.83203125" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="18.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="2" customWidth="1"/>
+    <col min="19" max="19" width="24.5" style="2" customWidth="1"/>
+    <col min="20" max="20" width="18" style="2" customWidth="1"/>
+    <col min="21" max="21" width="42.83203125" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1045,123 +1041,121 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" ht="102" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="O2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" ht="102" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="N3" s="2" t="str">
-        <f>TRIM(IF($H3="",$G3,"")
-&amp;IF($H3&lt;&gt;"",$H3,"")
-&amp;IF($I3&lt;&gt;""," "&amp;$I3,"")
-&amp;IF(OR($I3="LT",$I3="ST",AND($D3="",$I3&lt;&gt;"")),"-pos","")
-&amp;IF($K3&lt;&gt;""," "&amp;$K3,"")
-&amp;IF($J3&lt;&gt;""," "&amp;$J3&amp;"-pos","")
-&amp;IF($L3&lt;&gt;""," "&amp;$L3&amp;"-neg","")
+        <f>TRIM(IF($G3="",$F3,"")
+&amp;IF($G3&lt;&gt;"",$G3,"")
+&amp;IF($H3&lt;&gt;""," "&amp;$H3,"")
+&amp;IF(OR($H3="LT",$H3="ST"),"-pos","")
+&amp;IF($J3&lt;&gt;""," "&amp;$J3,"")
+&amp;IF($I3&lt;&gt;""," "&amp;$I3&amp;"-pos","")
+&amp;IF($K3&lt;&gt;""," "&amp;$K3&amp;"-neg","")
 &amp;", by "&amp;$C3&amp;" result")</f>
         <v>Dengue, by TAC result</v>
       </c>
       <c r="O3" s="2" t="str">
-        <f>TRIM("Raw "&amp;LOWER($E3)&amp;" data for "&amp;$B3)</f>
+        <f>TRIM("Raw "&amp;LOWER($D3)&amp;" data for "&amp;$B3)</f>
         <v>Raw virus data for stool</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="81" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:23" ht="106" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:23" ht="101" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:23" ht="94" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="81" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:22" ht="106" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:22" ht="101" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:22" ht="94" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:22" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="94" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>